<commit_message>
Let's add number to the test
</commit_message>
<xml_diff>
--- a/ExcelORM/ExcelORMTests/testFiles/first.xlsx
+++ b/ExcelORM/ExcelORMTests/testFiles/first.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576B8E84-A77D-4B7D-A846-F882AA9CA363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>First name</t>
   </si>
@@ -48,38 +57,25 @@
   <si>
     <t>Writer</t>
   </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,38 +84,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -146,21 +121,6 @@
       </right>
       <top style="thin">
         <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -199,42 +159,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -245,26 +199,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -466,7 +479,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -484,7 +497,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -513,7 +526,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -538,7 +551,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -563,7 +576,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -588,7 +601,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -613,7 +626,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -638,7 +651,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -663,7 +676,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -688,7 +701,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -713,7 +726,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -726,9 +739,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -745,7 +764,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -763,7 +782,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -788,7 +807,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -813,7 +832,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +857,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -863,7 +882,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -888,7 +907,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -913,7 +932,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -938,7 +957,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -963,7 +982,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -988,7 +1007,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1001,9 +1020,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1017,7 +1042,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1035,7 +1060,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1064,7 +1089,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,7 +1114,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1114,7 +1139,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1139,7 +1164,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1164,7 +1189,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1189,7 +1214,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1214,7 +1239,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1264,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1264,7 +1289,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,244 +1302,238 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+    <row r="1" spans="1:6" ht="20.25" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="4">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" t="s" s="7">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s" s="8">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="8">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" t="s" s="7">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s" s="7">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s" s="8">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s" s="8">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="6"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="6"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-    </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-    </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-    </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-    </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>